<commit_message>
Added debounce caps, Swapped USB connector to MINI, Updated Parts List
</commit_message>
<xml_diff>
--- a/lidar-breakout/PartsList_LidarBreakout.xlsx
+++ b/lidar-breakout/PartsList_LidarBreakout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akeen\Documents\GitHub\roboracing-electrical\lidar-breakout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF202EA-BABF-4778-A587-E841D76375AA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB42242-86D0-44A7-8D65-878744614C1E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="1430" windowHeight="4470" xr2:uid="{F5B95C38-B208-4F09-9CB9-CFEFED4EB7A5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{F5B95C38-B208-4F09-9CB9-CFEFED4EB7A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="118">
   <si>
     <t xml:space="preserve">WM1860-ND </t>
   </si>
@@ -216,15 +216,6 @@
     <t>Diodes Incorporated</t>
   </si>
   <si>
-    <t>P15097CT-ND</t>
-  </si>
-  <si>
-    <t>EEE-FTJ681XAP</t>
-  </si>
-  <si>
-    <t>CAP ALUM 680UF 20% 6.3V SMD</t>
-  </si>
-  <si>
     <t>1528-1104-ND</t>
   </si>
   <si>
@@ -306,18 +297,6 @@
     <t>PTC RESET FUSE 30V 200MA 1206</t>
   </si>
   <si>
-    <t>A97799DKR-ND</t>
-  </si>
-  <si>
-    <t>TE Connectivity AMP Connectors</t>
-  </si>
-  <si>
-    <t>1981584-1</t>
-  </si>
-  <si>
-    <t>CONN RCPT USB2.0 MICRO AB SMD RA</t>
-  </si>
-  <si>
     <t>507-1806-1-ND</t>
   </si>
   <si>
@@ -352,6 +331,60 @@
   </si>
   <si>
     <t>ORDER Quantities</t>
+  </si>
+  <si>
+    <t>P15367CT-ND</t>
+  </si>
+  <si>
+    <t>EEU-FR1E681LB</t>
+  </si>
+  <si>
+    <t>CAP ALUM 680UF 20% 25V RADIAL</t>
+  </si>
+  <si>
+    <t>H2960CT-ND</t>
+  </si>
+  <si>
+    <t>Hirose Electric Co Ltd</t>
+  </si>
+  <si>
+    <t>UX60-MB-5S8</t>
+  </si>
+  <si>
+    <t>CONN RCPT USB2.0 MINI B SMD R/A</t>
+  </si>
+  <si>
+    <t>BSS84PH6433XTMA1CT-ND</t>
+  </si>
+  <si>
+    <t>Infineon Technologies</t>
+  </si>
+  <si>
+    <t>BSS84PH6433XTMA1</t>
+  </si>
+  <si>
+    <t>MOSFET P-CH 60V 170MA SOT-23</t>
+  </si>
+  <si>
+    <t>490-9961-1-ND</t>
+  </si>
+  <si>
+    <t>GRM21BR61A476ME15L</t>
+  </si>
+  <si>
+    <t>CAP CER 47UF 10V X5R 0805</t>
+  </si>
+  <si>
+    <t>Murata Electronics North America</t>
+  </si>
+  <si>
+    <t>1276-1168-1-ND</t>
+  </si>
+  <si>
+    <t>CL10C471JB8NNNC</t>
+  </si>
+  <si>
+    <t>CAP CER 470PF 50V C0G/NP0 0603</t>
   </si>
 </sst>
 </file>
@@ -423,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -444,10 +477,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -456,33 +485,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="8" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -802,50 +813,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8667BB4C-F033-4764-83CB-DCC47EE63DF3}">
-  <dimension ref="A2:K44"/>
+  <dimension ref="A2:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C18" workbookViewId="0">
-      <selection activeCell="K31" sqref="K1:K31"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.90625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.90625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="6" customWidth="1"/>
-    <col min="4" max="4" width="6.36328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.36328125" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.26953125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44.36328125" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.26953125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.7265625" style="13"/>
-    <col min="11" max="11" width="17" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.7265625" style="13"/>
+    <col min="6" max="6" width="28.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.36328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.7265625" style="11"/>
+    <col min="11" max="11" width="17" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="11"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="10" t="s">
         <v>7</v>
       </c>
     </row>
@@ -859,7 +870,7 @@
       <c r="C3" s="6">
         <v>1</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="9">
         <v>0.96</v>
       </c>
       <c r="E3" s="3">
@@ -871,10 +882,10 @@
       <c r="G3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="15">
+      <c r="H3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="12">
         <f t="shared" ref="I3:I6" si="0">D3*C3</f>
         <v>0.96</v>
       </c>
@@ -890,7 +901,7 @@
       <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="9">
         <v>0.33</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -902,10 +913,10 @@
       <c r="G4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="15">
+      <c r="H4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="12">
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
@@ -921,7 +932,7 @@
       <c r="C5" s="6">
         <v>2</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="9">
         <v>0.16</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -933,10 +944,10 @@
       <c r="G5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="15">
+      <c r="H5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" s="12">
         <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
@@ -952,7 +963,7 @@
       <c r="C6" s="2">
         <v>6</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <v>0.17</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -964,10 +975,10 @@
       <c r="G6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6" s="15">
+      <c r="H6" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="12">
         <f t="shared" si="0"/>
         <v>1.02</v>
       </c>
@@ -983,7 +994,7 @@
       <c r="C7" s="2">
         <v>36</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="9">
         <v>0.11</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -995,10 +1006,10 @@
       <c r="G7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I7" s="15">
+      <c r="H7" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="12">
         <f>D7*C7</f>
         <v>3.96</v>
       </c>
@@ -1014,7 +1025,7 @@
       <c r="C8" s="2">
         <v>6</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="9">
         <v>0.56000000000000005</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -1026,18 +1037,18 @@
       <c r="G8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I8" s="15">
-        <f t="shared" ref="I8:I31" si="1">D8*C8</f>
+      <c r="H8" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="12">
+        <f t="shared" ref="I8:I34" si="1">D8*C8</f>
         <v>3.3600000000000003</v>
       </c>
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B9" s="2">
         <v>3</v>
@@ -1045,150 +1056,150 @@
       <c r="C9" s="2">
         <v>1</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="14">
         <v>0.21</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F9" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="15">
+      <c r="H9" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="12">
         <f>D9*C9</f>
         <v>0.21</v>
       </c>
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" s="10">
+      <c r="A10" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="8">
         <v>18</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="8">
         <v>6</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="14">
         <v>0.13</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I10" s="15">
+        <v>86</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="12">
         <f t="shared" si="1"/>
         <v>0.78</v>
       </c>
-      <c r="K10" s="10"/>
+      <c r="K10" s="8"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B11" s="10">
+        <v>88</v>
+      </c>
+      <c r="B11" s="8">
         <v>6</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="8">
         <v>2</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="15">
         <v>0.21</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I11" s="15">
+        <v>90</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="12">
         <f t="shared" si="1"/>
         <v>0.42</v>
       </c>
-      <c r="K11" s="10"/>
+      <c r="K11" s="8"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="10">
-        <v>3</v>
-      </c>
-      <c r="C12" s="10">
+        <v>103</v>
+      </c>
+      <c r="B12" s="8">
+        <v>3</v>
+      </c>
+      <c r="C12" s="8">
         <v>1</v>
       </c>
-      <c r="D12" s="19">
-        <v>0.45</v>
+      <c r="D12" s="15">
+        <v>0.99</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I12" s="15">
-        <f t="shared" si="1"/>
-        <v>0.45</v>
-      </c>
-      <c r="K12" s="10"/>
+        <v>104</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="12">
+        <f t="shared" si="1"/>
+        <v>0.99</v>
+      </c>
+      <c r="K12" s="8"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B13" s="10">
-        <v>3</v>
-      </c>
-      <c r="C13" s="10">
+        <v>92</v>
+      </c>
+      <c r="B13" s="8">
+        <v>3</v>
+      </c>
+      <c r="C13" s="8">
         <v>1</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="16">
         <v>0.36</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I13" s="15">
+        <v>93</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="12">
         <f t="shared" si="1"/>
         <v>0.36</v>
       </c>
-      <c r="K13" s="10"/>
+      <c r="K13" s="8"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -1200,7 +1211,7 @@
       <c r="C14" s="6">
         <v>1</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="9">
         <v>0.28999999999999998</v>
       </c>
       <c r="E14" s="6" t="s">
@@ -1212,10 +1223,10 @@
       <c r="G14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I14" s="15">
+      <c r="H14" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" s="12">
         <f t="shared" si="1"/>
         <v>0.28999999999999998</v>
       </c>
@@ -1231,7 +1242,7 @@
       <c r="C15" s="2">
         <v>3</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="9">
         <v>0.28999999999999998</v>
       </c>
       <c r="E15" s="2" t="s">
@@ -1243,10 +1254,10 @@
       <c r="G15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I15" s="15">
+      <c r="H15" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" s="12">
         <f t="shared" si="1"/>
         <v>0.86999999999999988</v>
       </c>
@@ -1262,7 +1273,7 @@
       <c r="C16" s="2">
         <v>6</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="9">
         <v>0.53</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -1274,17 +1285,17 @@
       <c r="G16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I16" s="15">
+      <c r="H16" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" s="12">
         <f t="shared" si="1"/>
         <v>3.18</v>
       </c>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="11" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="6">
@@ -1293,7 +1304,7 @@
       <c r="C17" s="6">
         <v>1</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="9">
         <v>1.95</v>
       </c>
       <c r="E17" s="2">
@@ -1302,13 +1313,13 @@
       <c r="F17" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I17" s="15">
+      <c r="H17" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" s="12">
         <f t="shared" si="1"/>
         <v>1.95</v>
       </c>
@@ -1324,7 +1335,7 @@
       <c r="C18" s="2">
         <v>2</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="9">
         <v>0.32</v>
       </c>
       <c r="E18" s="6" t="s">
@@ -1333,20 +1344,20 @@
       <c r="F18" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="H18" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I18" s="15">
+      <c r="H18" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I18" s="12">
         <f t="shared" si="1"/>
         <v>0.64</v>
       </c>
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="11" t="s">
         <v>42</v>
       </c>
       <c r="B19" s="6">
@@ -1355,7 +1366,7 @@
       <c r="C19" s="6">
         <v>12</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="9">
         <v>0.1</v>
       </c>
       <c r="E19" s="6" t="s">
@@ -1364,20 +1375,20 @@
       <c r="F19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I19" s="15">
+      <c r="H19" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" s="12">
         <f t="shared" si="1"/>
         <v>1.2000000000000002</v>
       </c>
       <c r="K19" s="6"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="11" t="s">
         <v>49</v>
       </c>
       <c r="B20" s="6">
@@ -1386,7 +1397,7 @@
       <c r="C20" s="6">
         <v>1</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="9">
         <v>0.92</v>
       </c>
       <c r="E20" s="6" t="s">
@@ -1395,20 +1406,20 @@
       <c r="F20" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="H20" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I20" s="15">
+      <c r="H20" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="12">
         <f t="shared" si="1"/>
         <v>0.92</v>
       </c>
       <c r="K20" s="6"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="11" t="s">
         <v>56</v>
       </c>
       <c r="B21" s="6">
@@ -1417,7 +1428,7 @@
       <c r="C21" s="6">
         <v>10</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="9">
         <v>0.1</v>
       </c>
       <c r="E21" s="6" t="s">
@@ -1426,20 +1437,20 @@
       <c r="F21" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="H21" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I21" s="15">
+      <c r="H21" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I21" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K21" s="6"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="11" t="s">
         <v>59</v>
       </c>
       <c r="B22" s="6">
@@ -1448,7 +1459,7 @@
       <c r="C22" s="6">
         <v>3</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="9">
         <v>0.44</v>
       </c>
       <c r="E22" s="6" t="s">
@@ -1457,21 +1468,21 @@
       <c r="F22" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="G22" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="H22" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I22" s="15">
+      <c r="H22" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I22" s="12">
         <f t="shared" si="1"/>
         <v>1.32</v>
       </c>
       <c r="K22" s="6"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>61</v>
+      <c r="A23" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="B23" s="6">
         <v>4</v>
@@ -1479,30 +1490,30 @@
       <c r="C23" s="6">
         <v>1</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="9">
         <v>0.8</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G23" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="H23" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I23" s="15">
+      <c r="G23" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23" s="12">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
       <c r="K23" s="6"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>64</v>
+      <c r="A24" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="B24" s="6">
         <v>3</v>
@@ -1510,7 +1521,7 @@
       <c r="C24" s="6">
         <v>1</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="12">
         <v>0.45</v>
       </c>
       <c r="E24" s="6">
@@ -1519,21 +1530,21 @@
       <c r="F24" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G24" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="H24" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I24" s="15">
+      <c r="G24" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I24" s="12">
         <f t="shared" si="1"/>
         <v>0.45</v>
       </c>
       <c r="K24" s="6"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>66</v>
+      <c r="A25" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="B25" s="6">
         <v>3</v>
@@ -1541,30 +1552,30 @@
       <c r="C25" s="6">
         <v>1</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="9">
         <v>4.12</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G25" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="H25" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I25" s="15">
+      <c r="G25" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" s="12">
         <f t="shared" si="1"/>
         <v>4.12</v>
       </c>
       <c r="K25" s="6"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>102</v>
+      <c r="A26" s="11" t="s">
+        <v>95</v>
       </c>
       <c r="B26" s="6">
         <v>6</v>
@@ -1572,30 +1583,30 @@
       <c r="C26" s="6">
         <v>2</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="9">
         <v>0.1</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="H26" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I26" s="15">
+      <c r="G26" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I26" s="12">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="K26" s="6"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
-        <v>69</v>
+      <c r="A27" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="B27" s="6">
         <v>6</v>
@@ -1603,30 +1614,30 @@
       <c r="C27" s="6">
         <v>2</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="9">
         <v>0.14000000000000001</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="H27" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I27" s="15">
+      <c r="G27" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="12">
         <f t="shared" si="1"/>
         <v>0.28000000000000003</v>
       </c>
       <c r="K27" s="6"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>72</v>
+      <c r="A28" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="B28" s="6">
         <v>6</v>
@@ -1634,30 +1645,30 @@
       <c r="C28" s="6">
         <v>2</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D28" s="9">
         <v>0.27</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G28" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I28" s="15">
+      <c r="G28" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I28" s="12">
         <f t="shared" si="1"/>
         <v>0.54</v>
       </c>
       <c r="K28" s="6"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>76</v>
+      <c r="A29" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="B29" s="6">
         <v>3</v>
@@ -1665,22 +1676,22 @@
       <c r="C29" s="6">
         <v>1</v>
       </c>
-      <c r="D29" s="15">
+      <c r="D29" s="12">
         <v>0.1</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G29" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="H29" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I29" s="15">
+      <c r="G29" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I29" s="12">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
@@ -1688,7 +1699,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B30" s="6">
         <v>10</v>
@@ -1696,30 +1707,30 @@
       <c r="C30" s="6">
         <v>3</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="9">
         <v>0.1</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G30" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I30" s="15">
+      <c r="G30" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I30" s="12">
         <f t="shared" si="1"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K30" s="6"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
-        <v>81</v>
+      <c r="A31" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="B31" s="6">
         <v>6</v>
@@ -1727,138 +1738,178 @@
       <c r="C31" s="6">
         <v>2</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="9">
         <v>0.1</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G31" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I31" s="15">
+      <c r="G31" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I31" s="12">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="K31" s="6"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I32" s="15"/>
+      <c r="A32" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" s="6">
+        <v>3</v>
+      </c>
+      <c r="C32" s="6">
+        <v>1</v>
+      </c>
+      <c r="D32" s="9">
+        <v>0.39</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I32" s="12">
+        <f t="shared" si="1"/>
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B33" s="6">
+        <v>3</v>
+      </c>
+      <c r="C33" s="6">
+        <v>1</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0.75</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I33" s="12">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H34" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="I34" s="15">
-        <f>SUM(I3:I31)</f>
-        <v>30.53</v>
+      <c r="A34" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" s="6">
+        <v>3</v>
+      </c>
+      <c r="C34" s="6">
+        <v>1</v>
+      </c>
+      <c r="D34" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I34" s="12">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="23"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
+      <c r="A35" s="1"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="7"/>
+      <c r="I35" s="12"/>
     </row>
     <row r="37" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="24"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="18"/>
+      <c r="A37" s="4"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="3"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="11"/>
     </row>
     <row r="38" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="24"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="18"/>
+      <c r="A38" s="4"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="3"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="11"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
+      <c r="A39" s="4"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="2"/>
+      <c r="G39" s="1"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="24"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
+      <c r="A40" s="4"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="4"/>
+      <c r="G40" s="1"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="24"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
+      <c r="A41" s="4"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="2"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="I41" s="12">
+        <f>SUM(I3:I32)</f>
+        <v>31.46</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="20"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
+      <c r="A42" s="1"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="1"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
+      <c r="A43" s="1"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="1"/>
+      <c r="G43" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
WIP - Rerouting Headers
</commit_message>
<xml_diff>
--- a/lidar-breakout/PartsList_LidarBreakout.xlsx
+++ b/lidar-breakout/PartsList_LidarBreakout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akeen\Documents\GitHub\roboracing-electrical\lidar-breakout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB42242-86D0-44A7-8D65-878744614C1E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0BC13A-78EA-4BE6-A0F5-291B536704B8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{F5B95C38-B208-4F09-9CB9-CFEFED4EB7A5}"/>
   </bookViews>
@@ -96,9 +96,6 @@
     <t xml:space="preserve">SSHL-002T-P0.2 </t>
   </si>
   <si>
-    <t xml:space="preserve">455-1582-1-ND </t>
-  </si>
-  <si>
     <t>JST</t>
   </si>
   <si>
@@ -385,6 +382,9 @@
   </si>
   <si>
     <t>CAP CER 470PF 50V C0G/NP0 0603</t>
+  </si>
+  <si>
+    <t>455-1568-1-ND</t>
   </si>
 </sst>
 </file>
@@ -815,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8667BB4C-F033-4764-83CB-DCC47EE63DF3}">
   <dimension ref="A2:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -839,13 +839,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>41</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>8</v>
@@ -970,7 +970,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>17</v>
@@ -1001,7 +1001,7 @@
         <v>20</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>19</v>
@@ -1017,7 +1017,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>21</v>
+        <v>117</v>
       </c>
       <c r="B8" s="2">
         <v>18</v>
@@ -1029,13 +1029,13 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>3</v>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B9" s="2">
         <v>3</v>
@@ -1060,13 +1060,13 @@
         <v>0.21</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>3</v>
@@ -1079,7 +1079,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" s="8">
         <v>18</v>
@@ -1091,13 +1091,13 @@
         <v>0.13</v>
       </c>
       <c r="E10" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>3</v>
@@ -1110,7 +1110,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B11" s="8">
         <v>6</v>
@@ -1122,13 +1122,13 @@
         <v>0.21</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>3</v>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B12" s="8">
         <v>3</v>
@@ -1153,13 +1153,13 @@
         <v>0.99</v>
       </c>
       <c r="E12" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>3</v>
@@ -1172,7 +1172,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B13" s="8">
         <v>3</v>
@@ -1184,13 +1184,13 @@
         <v>0.36</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>3</v>
@@ -1203,7 +1203,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="6">
         <v>3</v>
@@ -1215,13 +1215,13 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="E14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="H14" s="11" t="s">
         <v>3</v>
@@ -1234,7 +1234,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2">
         <v>8</v>
@@ -1246,13 +1246,13 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H15" s="11" t="s">
         <v>3</v>
@@ -1265,7 +1265,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="2">
         <v>15</v>
@@ -1277,13 +1277,13 @@
         <v>0.53</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H16" s="11" t="s">
         <v>3</v>
@@ -1296,7 +1296,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="6">
         <v>3</v>
@@ -1311,10 +1311,10 @@
         <v>3643</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H17" s="11" t="s">
         <v>3</v>
@@ -1327,7 +1327,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2">
         <v>6</v>
@@ -1339,13 +1339,13 @@
         <v>0.32</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>38</v>
       </c>
       <c r="H18" s="11" t="s">
         <v>3</v>
@@ -1358,7 +1358,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="6">
         <v>32</v>
@@ -1370,13 +1370,13 @@
         <v>0.1</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H19" s="11" t="s">
         <v>3</v>
@@ -1389,7 +1389,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="6">
         <v>3</v>
@@ -1401,13 +1401,13 @@
         <v>0.92</v>
       </c>
       <c r="E20" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="G20" s="11" t="s">
         <v>51</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>52</v>
       </c>
       <c r="H20" s="11" t="s">
         <v>3</v>
@@ -1420,7 +1420,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" s="6">
         <v>23</v>
@@ -1432,13 +1432,13 @@
         <v>0.1</v>
       </c>
       <c r="E21" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="G21" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H21" s="11" t="s">
         <v>3</v>
@@ -1451,7 +1451,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="6">
         <v>9</v>
@@ -1463,13 +1463,13 @@
         <v>0.44</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H22" s="11" t="s">
         <v>3</v>
@@ -1482,7 +1482,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B23" s="6">
         <v>4</v>
@@ -1494,13 +1494,13 @@
         <v>0.8</v>
       </c>
       <c r="E23" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" s="11" t="s">
         <v>101</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>102</v>
       </c>
       <c r="H23" s="11" t="s">
         <v>3</v>
@@ -1513,7 +1513,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24" s="6">
         <v>3</v>
@@ -1528,10 +1528,10 @@
         <v>1655</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H24" s="11" t="s">
         <v>3</v>
@@ -1544,7 +1544,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B25" s="6">
         <v>3</v>
@@ -1556,13 +1556,13 @@
         <v>4.12</v>
       </c>
       <c r="E25" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G25" s="11" t="s">
         <v>64</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>65</v>
       </c>
       <c r="H25" s="11" t="s">
         <v>3</v>
@@ -1575,7 +1575,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" s="6">
         <v>6</v>
@@ -1587,13 +1587,13 @@
         <v>0.1</v>
       </c>
       <c r="E26" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" s="11" t="s">
         <v>96</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>97</v>
       </c>
       <c r="H26" s="11" t="s">
         <v>3</v>
@@ -1606,7 +1606,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B27" s="6">
         <v>6</v>
@@ -1618,13 +1618,13 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H27" s="11" t="s">
         <v>3</v>
@@ -1637,7 +1637,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" s="6">
         <v>6</v>
@@ -1649,13 +1649,13 @@
         <v>0.27</v>
       </c>
       <c r="E28" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G28" s="11" t="s">
         <v>70</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>71</v>
       </c>
       <c r="H28" s="11" t="s">
         <v>3</v>
@@ -1668,7 +1668,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B29" s="6">
         <v>3</v>
@@ -1680,13 +1680,13 @@
         <v>0.1</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H29" s="11" t="s">
         <v>3</v>
@@ -1699,7 +1699,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B30" s="6">
         <v>10</v>
@@ -1711,13 +1711,13 @@
         <v>0.1</v>
       </c>
       <c r="E30" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G30" s="11" t="s">
         <v>76</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>77</v>
       </c>
       <c r="H30" s="11" t="s">
         <v>3</v>
@@ -1730,7 +1730,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B31" s="6">
         <v>6</v>
@@ -1742,13 +1742,13 @@
         <v>0.1</v>
       </c>
       <c r="E31" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G31" s="11" t="s">
         <v>79</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>80</v>
       </c>
       <c r="H31" s="11" t="s">
         <v>3</v>
@@ -1761,7 +1761,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B32" s="6">
         <v>3</v>
@@ -1773,13 +1773,13 @@
         <v>0.39</v>
       </c>
       <c r="E32" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="G32" s="11" t="s">
         <v>109</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>110</v>
       </c>
       <c r="H32" s="11" t="s">
         <v>3</v>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B33" s="6">
         <v>3</v>
@@ -1803,13 +1803,13 @@
         <v>0.75</v>
       </c>
       <c r="E33" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G33" s="11" t="s">
         <v>112</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>113</v>
       </c>
       <c r="H33" s="11" t="s">
         <v>3</v>
@@ -1821,7 +1821,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B34" s="6">
         <v>3</v>
@@ -1833,13 +1833,13 @@
         <v>0.1</v>
       </c>
       <c r="E34" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G34" s="11" t="s">
         <v>116</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>117</v>
       </c>
       <c r="H34" s="11" t="s">
         <v>3</v>
@@ -1893,7 +1893,7 @@
       <c r="E41" s="2"/>
       <c r="G41" s="1"/>
       <c r="H41" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I41" s="12">
         <f>SUM(I3:I32)</f>

</xml_diff>

<commit_message>
Updated parts list, cleaned up folder
</commit_message>
<xml_diff>
--- a/lidar-breakout/PartsList_LidarBreakout.xlsx
+++ b/lidar-breakout/PartsList_LidarBreakout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akeen\Documents\GitHub\roboracing-electrical\lidar-breakout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0BC13A-78EA-4BE6-A0F5-291B536704B8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A554F3-B793-44D3-AAE4-897F48BAD46A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{F5B95C38-B208-4F09-9CB9-CFEFED4EB7A5}"/>
+    <workbookView xWindow="7630" yWindow="0" windowWidth="10140" windowHeight="6000" xr2:uid="{F5B95C38-B208-4F09-9CB9-CFEFED4EB7A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="122">
   <si>
     <t xml:space="preserve">WM1860-ND </t>
   </si>
@@ -385,16 +385,29 @@
   </si>
   <si>
     <t>455-1568-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EG4372-ND </t>
+  </si>
+  <si>
+    <t>TL1105XF160Q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWITCH TACTILE SPST-NO 0.05A 12V </t>
+  </si>
+  <si>
+    <t>E-Switch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,13 +416,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -426,6 +432,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -435,7 +460,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -443,20 +468,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -468,10 +485,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -481,26 +498,35 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="8" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -815,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8667BB4C-F033-4764-83CB-DCC47EE63DF3}">
   <dimension ref="A2:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -824,7 +850,7 @@
     <col min="1" max="1" width="22.90625" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="6" customWidth="1"/>
-    <col min="4" max="4" width="6.36328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.81640625" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.26953125" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="44.36328125" style="11" bestFit="1" customWidth="1"/>
@@ -1041,7 +1067,7 @@
         <v>3</v>
       </c>
       <c r="I8" s="12">
-        <f t="shared" ref="I8:I34" si="1">D8*C8</f>
+        <f t="shared" ref="I8:I35" si="1">D8*C8</f>
         <v>3.3600000000000003</v>
       </c>
       <c r="K8" s="2"/>
@@ -1056,7 +1082,7 @@
       <c r="C9" s="2">
         <v>1</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="13">
         <v>0.21</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -1087,7 +1113,7 @@
       <c r="C10" s="8">
         <v>6</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="13">
         <v>0.13</v>
       </c>
       <c r="E10" s="6" t="s">
@@ -1118,7 +1144,7 @@
       <c r="C11" s="8">
         <v>2</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="14">
         <v>0.21</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -1149,7 +1175,7 @@
       <c r="C12" s="8">
         <v>1</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="14">
         <v>0.99</v>
       </c>
       <c r="E12" s="6" t="s">
@@ -1180,7 +1206,7 @@
       <c r="C13" s="8">
         <v>1</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="15">
         <v>0.36</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -1330,10 +1356,10 @@
         <v>25</v>
       </c>
       <c r="B18" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C18" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="9">
         <v>0.32</v>
@@ -1352,7 +1378,7 @@
       </c>
       <c r="I18" s="12">
         <f t="shared" si="1"/>
-        <v>0.64</v>
+        <v>0.32</v>
       </c>
       <c r="K18" s="2"/>
     </row>
@@ -1849,13 +1875,35 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="7"/>
-      <c r="I35" s="12"/>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B35" s="18">
+        <v>3</v>
+      </c>
+      <c r="C35" s="2">
+        <v>1</v>
+      </c>
+      <c r="D35" s="19">
+        <v>0.32</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G35" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I35" s="12">
+        <f t="shared" si="1"/>
+        <v>0.32</v>
+      </c>
     </row>
     <row r="37" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
@@ -1892,12 +1940,12 @@
       <c r="D41" s="4"/>
       <c r="E41" s="2"/>
       <c r="G41" s="1"/>
-      <c r="H41" s="17" t="s">
+      <c r="H41" s="16" t="s">
         <v>97</v>
       </c>
       <c r="I41" s="12">
         <f>SUM(I3:I32)</f>
-        <v>31.46</v>
+        <v>31.14</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>